<commit_message>
update input spreadsheets and add new cases
</commit_message>
<xml_diff>
--- a/inputs/input spreadsheets/1-input_unmet_demand-cp0.xlsx
+++ b/inputs/input spreadsheets/1-input_unmet_demand-cp0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mengyao @ Carnegie\research\SEM models\projects\cost of unmet demand\SEM-1.1-unmet-demand-my190226\input spreadsheets\v4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Becca/Documents/Git/cost-of-unmet-demand/inputs/input spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B76627-915B-402E-86CA-4E5057CFFADE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119924F0-E82B-8444-9288-5C07F60A77C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25080" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EIAbase" sheetId="19" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -207,18 +209,6 @@
     <t>Scaling value for demand to increase accuracy of optimizer results. Ideally, should have no implication for final results.</t>
   </si>
   <si>
-    <t>Input_Data/Shaner-et-al_E&amp;ES2018</t>
-  </si>
-  <si>
-    <t>solar_series_Shaner_normalized_to_0.2_mean.csv</t>
-  </si>
-  <si>
-    <t>wind_series_Shaner_normalized_to_0.38_mean.csv</t>
-  </si>
-  <si>
-    <t>demand_series_Shaner_normalized_to_1_mean.csv</t>
-  </si>
-  <si>
     <t>PGP_STORAGE_CHARGING_EFFICIENCY</t>
   </si>
   <si>
@@ -409,6 +399,18 @@
   </si>
   <si>
     <t>1-unmet_demand-cp0</t>
+  </si>
+  <si>
+    <t>US_demand_unnormalized.csv</t>
+  </si>
+  <si>
+    <t>US_capacity_solar_threshold26_unnormalized.csv</t>
+  </si>
+  <si>
+    <t>US_capacity_wind_threshold26_unnormalized.csv</t>
+  </si>
+  <si>
+    <t>Input_Data/Lei_Solar_Wind</t>
   </si>
 </sst>
 </file>
@@ -1312,204 +1314,204 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528F748F-2438-463B-BA5E-87C8F32FAD91}">
   <dimension ref="A1:E226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="8" customWidth="1"/>
-    <col min="3" max="16384" width="12.5703125" style="1"/>
+    <col min="3" max="16384" width="12.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
     </row>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B6" s="8"/>
     </row>
-    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B7" s="8"/>
     </row>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="8"/>
     </row>
-    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="8"/>
     </row>
-    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="8"/>
     </row>
-    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="8"/>
     </row>
-    <row r="12" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B13" s="8"/>
     </row>
-    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="8"/>
     </row>
-    <row r="15" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="8"/>
     </row>
-    <row r="16" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
     </row>
-    <row r="17" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
     </row>
-    <row r="19" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
     </row>
-    <row r="22" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="8"/>
     </row>
-    <row r="24" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="8"/>
     </row>
-    <row r="25" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="8"/>
     </row>
-    <row r="26" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="8"/>
     </row>
-    <row r="30" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="8"/>
     </row>
-    <row r="31" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
     </row>
-    <row r="32" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="8"/>
     </row>
-    <row r="33" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="8"/>
     </row>
-    <row r="34" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>13</v>
       </c>
       <c r="B34" s="8"/>
     </row>
-    <row r="35" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B36" s="8"/>
     </row>
-    <row r="37" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>15</v>
       </c>
       <c r="B37" s="8"/>
     </row>
-    <row r="38" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="8"/>
     </row>
-    <row r="39" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="8"/>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>17</v>
       </c>
@@ -1517,29 +1519,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
       <c r="C44" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>21</v>
       </c>
@@ -1550,12 +1552,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="10"/>
       <c r="C46"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>24</v>
       </c>
@@ -1566,7 +1568,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>26</v>
       </c>
@@ -1577,21 +1579,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B49" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C52"/>
     </row>
-    <row r="53" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>30</v>
       </c>
@@ -1600,10 +1602,10 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C54"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>55</v>
       </c>
@@ -1614,7 +1616,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>56</v>
       </c>
@@ -1625,50 +1627,50 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="10"/>
       <c r="C57"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B58" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58"/>
+    </row>
+    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C58"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="B59" s="10" t="b">
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="10"/>
       <c r="C60"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B61" s="10">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="C61" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D61"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>34</v>
       </c>
@@ -1676,11 +1678,11 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D62"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>35</v>
       </c>
@@ -1688,11 +1690,11 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D63"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>36</v>
       </c>
@@ -1700,23 +1702,23 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D64"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B65" s="10">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="C65" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D65"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>38</v>
       </c>
@@ -1724,11 +1726,11 @@
         <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D66"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>39</v>
       </c>
@@ -1736,11 +1738,11 @@
         <v>31</v>
       </c>
       <c r="C67" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D67"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>40</v>
       </c>
@@ -1748,64 +1750,64 @@
         <v>24</v>
       </c>
       <c r="C68" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D68"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="10"/>
       <c r="C69"/>
       <c r="D69"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B70" s="10">
         <v>0</v>
       </c>
       <c r="C70" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D70"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="10"/>
       <c r="C71"/>
       <c r="D71"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="C72"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B73" s="13">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C73" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D73" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="E73" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B74" s="11">
         <f>0.00000001</f>
@@ -1816,70 +1818,70 @@
       </c>
       <c r="D74"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B75" s="10">
         <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D75" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B76" s="10">
         <v>0</v>
       </c>
       <c r="C76" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D76" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="10"/>
       <c r="C77"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="C78"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B79" s="13">
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C79" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D79" s="14">
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="E79" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B80" s="11">
         <v>1.05E-8</v>
@@ -1889,60 +1891,60 @@
       </c>
       <c r="D80"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B81" s="10">
         <v>0</v>
       </c>
       <c r="C81" t="s">
+        <v>102</v>
+      </c>
+      <c r="D81" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="D81" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="B82" s="10">
         <v>0</v>
       </c>
       <c r="C82" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D82" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="10"/>
       <c r="C83"/>
       <c r="D83"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B84" s="13">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C84" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D84" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="E84" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B85" s="13">
         <v>2.2590009128958689E-2</v>
@@ -1954,63 +1956,63 @@
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="E85" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B86" s="10">
         <v>0</v>
       </c>
       <c r="C86" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D86" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B87" s="12">
         <v>0.49</v>
       </c>
       <c r="C87" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D87" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
       <c r="B88" s="10"/>
       <c r="C88"/>
       <c r="D88"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B89" s="10">
         <v>-1</v>
       </c>
       <c r="C89" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D89" s="14">
         <v>2.7271220888813726E-2</v>
       </c>
       <c r="E89" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B90" s="10">
         <v>-1</v>
@@ -2022,63 +2024,63 @@
         <v>2.9679010772171249E-2</v>
       </c>
       <c r="E90" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B91" s="10">
         <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D91" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B92" s="12">
         <v>0.17</v>
       </c>
       <c r="C92" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D92" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="10"/>
       <c r="C93"/>
       <c r="D93"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B94" s="10">
         <v>-1</v>
       </c>
       <c r="C94" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D94" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="E94" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B95" s="10">
         <v>-1</v>
@@ -2090,82 +2092,82 @@
         <v>2.5158160216169324E-2</v>
       </c>
       <c r="E95" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B96" s="10">
         <v>0</v>
       </c>
       <c r="C96" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D96" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B97" s="10">
         <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D97" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="4"/>
       <c r="B98" s="10"/>
       <c r="C98"/>
       <c r="D98"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B99" s="13">
         <v>4.2392529406082022E-3</v>
       </c>
       <c r="C99" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D99" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B100" s="10">
         <v>0</v>
       </c>
       <c r="C100" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D100"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B101" s="10">
         <v>0</v>
       </c>
       <c r="C101" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D101"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>46</v>
       </c>
@@ -2175,7 +2177,7 @@
       <c r="C102"/>
       <c r="D102"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>47</v>
       </c>
@@ -2188,10 +2190,10 @@
       </c>
       <c r="D103"/>
       <c r="E103" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>49</v>
       </c>
@@ -2202,88 +2204,88 @@
         <v>50</v>
       </c>
       <c r="D104" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="4"/>
       <c r="B105" s="10"/>
       <c r="C105"/>
       <c r="D105"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B106" s="10">
         <v>-1</v>
       </c>
       <c r="C106" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D106" s="10">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="E106" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B107" s="10">
         <v>-1</v>
       </c>
       <c r="C107" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D107" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B108" s="10">
         <v>-1</v>
       </c>
       <c r="C108" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D108" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B109" s="10">
         <v>0</v>
       </c>
       <c r="C109" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D109"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B110" s="10">
         <v>0</v>
       </c>
       <c r="C110" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D110"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B111" s="10">
         <f>D111</f>
@@ -2297,12 +2299,12 @@
         <v>1.1407453648359933E-8</v>
       </c>
       <c r="E111" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B112" s="10">
         <v>0.3</v>
@@ -2310,53 +2312,53 @@
       <c r="C112"/>
       <c r="D112"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="4"/>
       <c r="B113" s="10"/>
       <c r="C113"/>
       <c r="D113"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B114" s="10">
         <v>1</v>
       </c>
       <c r="C114" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D114"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C115" s="8"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C116" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" spans="1:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B119" s="1"/>
     </row>
-    <row r="120" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="str">
         <f>"exp" &amp; TEXT(D120,"0.00")</f>
         <v>exp3.00</v>
@@ -2370,7 +2372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="15" t="str">
         <f t="shared" ref="A121:A155" si="0">"exp" &amp; TEXT(D121,"0.00")</f>
         <v>exp2.95</v>
@@ -2385,7 +2387,7 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="122" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.90</v>
@@ -2400,7 +2402,7 @@
         <v>2.9000000000000004</v>
       </c>
     </row>
-    <row r="123" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.85</v>
@@ -2415,7 +2417,7 @@
         <v>2.8500000000000005</v>
       </c>
     </row>
-    <row r="124" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.80</v>
@@ -2430,7 +2432,7 @@
         <v>2.8000000000000007</v>
       </c>
     </row>
-    <row r="125" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.75</v>
@@ -2445,7 +2447,7 @@
         <v>2.7500000000000009</v>
       </c>
     </row>
-    <row r="126" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.70</v>
@@ -2460,7 +2462,7 @@
         <v>2.7000000000000011</v>
       </c>
     </row>
-    <row r="127" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.65</v>
@@ -2475,7 +2477,7 @@
         <v>2.6500000000000012</v>
       </c>
     </row>
-    <row r="128" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.60</v>
@@ -2490,7 +2492,7 @@
         <v>2.6000000000000014</v>
       </c>
     </row>
-    <row r="129" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.55</v>
@@ -2505,7 +2507,7 @@
         <v>2.5500000000000016</v>
       </c>
     </row>
-    <row r="130" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.50</v>
@@ -2520,7 +2522,7 @@
         <v>2.5000000000000018</v>
       </c>
     </row>
-    <row r="131" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.45</v>
@@ -2535,7 +2537,7 @@
         <v>2.450000000000002</v>
       </c>
     </row>
-    <row r="132" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.40</v>
@@ -2550,7 +2552,7 @@
         <v>2.4000000000000021</v>
       </c>
     </row>
-    <row r="133" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.35</v>
@@ -2565,7 +2567,7 @@
         <v>2.3500000000000023</v>
       </c>
     </row>
-    <row r="134" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.30</v>
@@ -2580,7 +2582,7 @@
         <v>2.3000000000000025</v>
       </c>
     </row>
-    <row r="135" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.25</v>
@@ -2595,7 +2597,7 @@
         <v>2.2500000000000027</v>
       </c>
     </row>
-    <row r="136" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.20</v>
@@ -2610,7 +2612,7 @@
         <v>2.2000000000000028</v>
       </c>
     </row>
-    <row r="137" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.15</v>
@@ -2625,7 +2627,7 @@
         <v>2.150000000000003</v>
       </c>
     </row>
-    <row r="138" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.10</v>
@@ -2640,7 +2642,7 @@
         <v>2.1000000000000032</v>
       </c>
     </row>
-    <row r="139" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.05</v>
@@ -2655,7 +2657,7 @@
         <v>2.0500000000000034</v>
       </c>
     </row>
-    <row r="140" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp2.00</v>
@@ -2670,7 +2672,7 @@
         <v>2.0000000000000036</v>
       </c>
     </row>
-    <row r="141" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.95</v>
@@ -2685,7 +2687,7 @@
         <v>1.9500000000000035</v>
       </c>
     </row>
-    <row r="142" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.90</v>
@@ -2700,7 +2702,7 @@
         <v>1.9000000000000035</v>
       </c>
     </row>
-    <row r="143" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.85</v>
@@ -2715,7 +2717,7 @@
         <v>1.8500000000000034</v>
       </c>
     </row>
-    <row r="144" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.80</v>
@@ -2730,7 +2732,7 @@
         <v>1.8000000000000034</v>
       </c>
     </row>
-    <row r="145" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.75</v>
@@ -2745,7 +2747,7 @@
         <v>1.7500000000000033</v>
       </c>
     </row>
-    <row r="146" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.70</v>
@@ -2760,7 +2762,7 @@
         <v>1.7000000000000033</v>
       </c>
     </row>
-    <row r="147" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.65</v>
@@ -2775,7 +2777,7 @@
         <v>1.6500000000000032</v>
       </c>
     </row>
-    <row r="148" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.60</v>
@@ -2790,7 +2792,7 @@
         <v>1.6000000000000032</v>
       </c>
     </row>
-    <row r="149" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.55</v>
@@ -2805,7 +2807,7 @@
         <v>1.5500000000000032</v>
       </c>
     </row>
-    <row r="150" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.50</v>
@@ -2820,7 +2822,7 @@
         <v>1.5000000000000031</v>
       </c>
     </row>
-    <row r="151" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.45</v>
@@ -2835,7 +2837,7 @@
         <v>1.4500000000000031</v>
       </c>
     </row>
-    <row r="152" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.40</v>
@@ -2850,7 +2852,7 @@
         <v>1.400000000000003</v>
       </c>
     </row>
-    <row r="153" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.35</v>
@@ -2865,7 +2867,7 @@
         <v>1.350000000000003</v>
       </c>
     </row>
-    <row r="154" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.30</v>
@@ -2880,7 +2882,7 @@
         <v>1.3000000000000029</v>
       </c>
     </row>
-    <row r="155" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="15" t="str">
         <f t="shared" si="0"/>
         <v>exp1.25</v>
@@ -2895,7 +2897,7 @@
         <v>1.2500000000000029</v>
       </c>
     </row>
-    <row r="156" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="15" t="str">
         <f>"exp" &amp; TEXT(D156,"0.00")</f>
         <v>exp1.20</v>
@@ -2910,7 +2912,7 @@
         <v>1.2000000000000028</v>
       </c>
     </row>
-    <row r="157" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="15" t="str">
         <f t="shared" ref="A157:A179" si="3">"exp" &amp; TEXT(D157,"0.00")</f>
         <v>exp1.15</v>
@@ -2925,7 +2927,7 @@
         <v>1.1500000000000028</v>
       </c>
     </row>
-    <row r="158" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp1.10</v>
@@ -2940,7 +2942,7 @@
         <v>1.1000000000000028</v>
       </c>
     </row>
-    <row r="159" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp1.05</v>
@@ -2955,7 +2957,7 @@
         <v>1.0500000000000027</v>
       </c>
     </row>
-    <row r="160" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp1.00</v>
@@ -2970,7 +2972,7 @@
         <v>1.0000000000000027</v>
       </c>
     </row>
-    <row r="161" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.95</v>
@@ -2985,7 +2987,7 @@
         <v>0.95000000000000262</v>
       </c>
     </row>
-    <row r="162" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.90</v>
@@ -3000,7 +3002,7 @@
         <v>0.90000000000000258</v>
       </c>
     </row>
-    <row r="163" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.85</v>
@@ -3015,7 +3017,7 @@
         <v>0.85000000000000253</v>
       </c>
     </row>
-    <row r="164" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.80</v>
@@ -3030,7 +3032,7 @@
         <v>0.80000000000000249</v>
       </c>
     </row>
-    <row r="165" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.75</v>
@@ -3045,7 +3047,7 @@
         <v>0.75000000000000244</v>
       </c>
     </row>
-    <row r="166" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.70</v>
@@ -3060,7 +3062,7 @@
         <v>0.7000000000000024</v>
       </c>
     </row>
-    <row r="167" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.65</v>
@@ -3075,7 +3077,7 @@
         <v>0.65000000000000235</v>
       </c>
     </row>
-    <row r="168" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.60</v>
@@ -3090,7 +3092,7 @@
         <v>0.60000000000000231</v>
       </c>
     </row>
-    <row r="169" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.55</v>
@@ -3105,7 +3107,7 @@
         <v>0.55000000000000226</v>
       </c>
     </row>
-    <row r="170" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.50</v>
@@ -3120,7 +3122,7 @@
         <v>0.50000000000000222</v>
       </c>
     </row>
-    <row r="171" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A171" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.45</v>
@@ -3135,7 +3137,7 @@
         <v>0.45000000000000223</v>
       </c>
     </row>
-    <row r="172" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.40</v>
@@ -3150,7 +3152,7 @@
         <v>0.40000000000000224</v>
       </c>
     </row>
-    <row r="173" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.35</v>
@@ -3165,7 +3167,7 @@
         <v>0.35000000000000225</v>
       </c>
     </row>
-    <row r="174" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.30</v>
@@ -3180,7 +3182,7 @@
         <v>0.30000000000000226</v>
       </c>
     </row>
-    <row r="175" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.25</v>
@@ -3195,7 +3197,7 @@
         <v>0.25000000000000228</v>
       </c>
     </row>
-    <row r="176" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.20</v>
@@ -3210,7 +3212,7 @@
         <v>0.20000000000000229</v>
       </c>
     </row>
-    <row r="177" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A177" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.15</v>
@@ -3225,7 +3227,7 @@
         <v>0.1500000000000023</v>
       </c>
     </row>
-    <row r="178" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A178" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.10</v>
@@ -3240,7 +3242,7 @@
         <v>0.1000000000000023</v>
       </c>
     </row>
-    <row r="179" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A179" s="15" t="str">
         <f t="shared" si="3"/>
         <v>exp0.05</v>
@@ -3255,7 +3257,7 @@
         <v>5.0000000000002293E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A180" s="15" t="str">
         <f>"exp" &amp; TEXT(D180,"0.00")</f>
         <v>exp0.00</v>
@@ -3269,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A181" s="15" t="str">
         <f t="shared" ref="A181:A215" si="5">"exp" &amp; TEXT(D181,"0.00")</f>
         <v>exp-0.05</v>
@@ -3284,7 +3286,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="182" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A182" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.10</v>
@@ -3299,7 +3301,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="183" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A183" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.15</v>
@@ -3314,7 +3316,7 @@
         <v>-0.15000000000000002</v>
       </c>
     </row>
-    <row r="184" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.20</v>
@@ -3329,7 +3331,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="185" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.25</v>
@@ -3344,7 +3346,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="186" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A186" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.30</v>
@@ -3359,7 +3361,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="187" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.35</v>
@@ -3374,7 +3376,7 @@
         <v>-0.35</v>
       </c>
     </row>
-    <row r="188" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A188" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.40</v>
@@ -3389,7 +3391,7 @@
         <v>-0.39999999999999997</v>
       </c>
     </row>
-    <row r="189" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.45</v>
@@ -3404,7 +3406,7 @@
         <v>-0.44999999999999996</v>
       </c>
     </row>
-    <row r="190" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.50</v>
@@ -3419,7 +3421,7 @@
         <v>-0.49999999999999994</v>
       </c>
     </row>
-    <row r="191" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A191" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.55</v>
@@ -3434,7 +3436,7 @@
         <v>-0.54999999999999993</v>
       </c>
     </row>
-    <row r="192" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.60</v>
@@ -3449,7 +3451,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="193" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.65</v>
@@ -3464,7 +3466,7 @@
         <v>-0.65</v>
       </c>
     </row>
-    <row r="194" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.70</v>
@@ -3479,7 +3481,7 @@
         <v>-0.70000000000000007</v>
       </c>
     </row>
-    <row r="195" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.75</v>
@@ -3494,7 +3496,7 @@
         <v>-0.75000000000000011</v>
       </c>
     </row>
-    <row r="196" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.80</v>
@@ -3509,7 +3511,7 @@
         <v>-0.80000000000000016</v>
       </c>
     </row>
-    <row r="197" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A197" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.85</v>
@@ -3524,7 +3526,7 @@
         <v>-0.8500000000000002</v>
       </c>
     </row>
-    <row r="198" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.90</v>
@@ -3539,13 +3541,13 @@
         <v>-0.90000000000000024</v>
       </c>
     </row>
-    <row r="199" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-0.95</v>
       </c>
       <c r="B199" s="16">
-        <f t="shared" si="6"/>
+        <f>10^D199</f>
         <v>0.11220184543019628</v>
       </c>
       <c r="C199" s="15"/>
@@ -3554,7 +3556,7 @@
         <v>-0.95000000000000029</v>
       </c>
     </row>
-    <row r="200" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.00</v>
@@ -3569,7 +3571,7 @@
         <v>-1.0000000000000002</v>
       </c>
     </row>
-    <row r="201" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.05</v>
@@ -3584,7 +3586,7 @@
         <v>-1.0500000000000003</v>
       </c>
     </row>
-    <row r="202" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.10</v>
@@ -3599,7 +3601,7 @@
         <v>-1.1000000000000003</v>
       </c>
     </row>
-    <row r="203" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A203" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.15</v>
@@ -3614,7 +3616,7 @@
         <v>-1.1500000000000004</v>
       </c>
     </row>
-    <row r="204" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.20</v>
@@ -3629,7 +3631,7 @@
         <v>-1.2000000000000004</v>
       </c>
     </row>
-    <row r="205" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A205" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.25</v>
@@ -3644,7 +3646,7 @@
         <v>-1.2500000000000004</v>
       </c>
     </row>
-    <row r="206" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.30</v>
@@ -3659,7 +3661,7 @@
         <v>-1.3000000000000005</v>
       </c>
     </row>
-    <row r="207" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A207" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.35</v>
@@ -3674,7 +3676,7 @@
         <v>-1.3500000000000005</v>
       </c>
     </row>
-    <row r="208" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.40</v>
@@ -3689,7 +3691,7 @@
         <v>-1.4000000000000006</v>
       </c>
     </row>
-    <row r="209" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A209" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.45</v>
@@ -3704,7 +3706,7 @@
         <v>-1.4500000000000006</v>
       </c>
     </row>
-    <row r="210" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.50</v>
@@ -3719,7 +3721,7 @@
         <v>-1.5000000000000007</v>
       </c>
     </row>
-    <row r="211" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A211" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.55</v>
@@ -3734,7 +3736,7 @@
         <v>-1.5500000000000007</v>
       </c>
     </row>
-    <row r="212" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A212" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.60</v>
@@ -3749,7 +3751,7 @@
         <v>-1.6000000000000008</v>
       </c>
     </row>
-    <row r="213" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A213" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.65</v>
@@ -3764,7 +3766,7 @@
         <v>-1.6500000000000008</v>
       </c>
     </row>
-    <row r="214" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A214" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.70</v>
@@ -3779,7 +3781,7 @@
         <v>-1.7000000000000008</v>
       </c>
     </row>
-    <row r="215" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A215" s="15" t="str">
         <f t="shared" si="5"/>
         <v>exp-1.75</v>
@@ -3794,7 +3796,7 @@
         <v>-1.7500000000000009</v>
       </c>
     </row>
-    <row r="216" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A216" s="15" t="str">
         <f>"exp" &amp; TEXT(D216,"0.00")</f>
         <v>exp-1.80</v>
@@ -3809,7 +3811,7 @@
         <v>-1.8000000000000009</v>
       </c>
     </row>
-    <row r="217" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217" s="15" t="str">
         <f t="shared" ref="A217:A220" si="10">"exp" &amp; TEXT(D217,"0.00")</f>
         <v>exp-1.85</v>
@@ -3824,7 +3826,7 @@
         <v>-1.850000000000001</v>
       </c>
     </row>
-    <row r="218" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218" s="15" t="str">
         <f t="shared" si="10"/>
         <v>exp-1.90</v>
@@ -3839,7 +3841,7 @@
         <v>-1.900000000000001</v>
       </c>
     </row>
-    <row r="219" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A219" s="15" t="str">
         <f t="shared" si="10"/>
         <v>exp-1.95</v>
@@ -3854,7 +3856,7 @@
         <v>-1.9500000000000011</v>
       </c>
     </row>
-    <row r="220" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A220" s="15" t="str">
         <f t="shared" si="10"/>
         <v>exp-2.00</v>
@@ -3869,13 +3871,13 @@
         <v>-2.0000000000000009</v>
       </c>
     </row>
-    <row r="222" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B222" s="9"/>
     </row>
-    <row r="226" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>